<commit_message>
Make week 26 team
</commit_message>
<xml_diff>
--- a/Predictions/2023-24/Week 25.xlsx
+++ b/Predictions/2023-24/Week 25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corridog/Documents/GitHub/FPL-Predictor/Predictions/2023-24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8F97CE-BCA4-2441-8BAC-96D54102DE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B145E28D-C0CE-BB4A-AB3A-F8378446CA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="33060" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1206,17 +1206,15 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AL157" totalsRowShown="0">
   <autoFilter ref="A1:AL157" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="36">
-      <filters>
-        <filter val="0"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="37">
       <filters>
         <filter val="1"/>
       </filters>
     </filterColumn>
   </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:AL143">
+    <sortCondition descending="1" ref="AI1:AI157"/>
+  </sortState>
   <tableColumns count="38">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="First Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Surname"/>
@@ -1551,7 +1549,7 @@
   <dimension ref="A1:AP157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C110" sqref="A110:C110"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1799,7 +1797,7 @@
       </c>
       <c r="AO2">
         <f>SUMPRODUCT(Table1[Selected], Table1[PP])</f>
-        <v>375.16553713381836</v>
+        <v>375.16553713381842</v>
       </c>
       <c r="AP2" t="s">
         <v>1</v>
@@ -2045,7 +2043,7 @@
       </c>
       <c r="AO4">
         <f>SUMPRODUCT(Table1[Selected],Table1[Cost])</f>
-        <v>97.4</v>
+        <v>97.399999999999991</v>
       </c>
       <c r="AP4">
         <v>101.9</v>
@@ -2425,36 +2423,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>266</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>267</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>267</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -2490,7 +2488,7 @@
         <v>0</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -2514,24 +2512,24 @@
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>5.6</v>
+        <v>14.4</v>
       </c>
       <c r="AE8">
-        <v>18</v>
+        <v>499</v>
       </c>
       <c r="AF8">
-        <v>18.217404566884401</v>
+        <v>47.510204081632637</v>
       </c>
       <c r="AG8">
-        <v>19.065496153059801</v>
+        <v>47.672769754447117</v>
       </c>
       <c r="AH8">
-        <f>20.4859392927446*1</f>
-        <v>20.4859392927446</v>
+        <f>55.5244687021735*1</f>
+        <v>55.5244687021735</v>
       </c>
       <c r="AI8">
-        <f>3.61005959840199*1</f>
-        <v>3.6100595984019899</v>
+        <f>18.5367479360317*1</f>
+        <v>18.536747936031698</v>
       </c>
       <c r="AJ8">
         <v>1</v>
@@ -3531,7 +3529,7 @@
       </c>
       <c r="AO16">
         <f>AO2-AO14*5</f>
-        <v>335.16553713381836</v>
+        <v>335.16553713381842</v>
       </c>
     </row>
     <row r="17" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
@@ -4548,24 +4546,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>241</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>242</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>242</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -4574,7 +4572,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -4583,7 +4581,7 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -4610,7 +4608,7 @@
         <v>0</v>
       </c>
       <c r="U25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V25">
         <v>0</v>
@@ -4640,27 +4638,27 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="AE25">
-        <v>92</v>
+        <v>450</v>
       </c>
       <c r="AF25">
-        <v>21.700584998227729</v>
+        <v>12.56844477409547</v>
       </c>
       <c r="AG25">
-        <v>19.416666666666671</v>
+        <v>17.749994511662958</v>
       </c>
       <c r="AH25">
-        <f>24.8022480203325*1</f>
-        <v>24.802248020332499</v>
+        <f>28.2252863204879*1</f>
+        <v>28.2252863204879</v>
       </c>
       <c r="AI25">
-        <f>4.09094795889088*1</f>
-        <v>4.0909479588908804</v>
+        <f>10.169834381442*1</f>
+        <v>10.169834381442</v>
       </c>
       <c r="AJ25">
         <v>1</v>
       </c>
       <c r="AK25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL25">
         <v>1</v>
@@ -5060,18 +5058,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>264</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>265</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>265</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -5080,13 +5078,13 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -5095,7 +5093,7 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -5125,7 +5123,7 @@
         <v>0</v>
       </c>
       <c r="V29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W29">
         <v>0</v>
@@ -5149,24 +5147,24 @@
         <v>0</v>
       </c>
       <c r="AD29">
-        <v>6.9</v>
+        <v>8</v>
       </c>
       <c r="AE29">
-        <v>100</v>
+        <v>497</v>
       </c>
       <c r="AF29">
-        <v>30.73863803650563</v>
+        <v>34.804013156453273</v>
       </c>
       <c r="AG29">
-        <v>17.131578947368421</v>
+        <v>24.474696445768739</v>
       </c>
       <c r="AH29">
-        <f>25.5109831822738*1</f>
-        <v>25.510983182273801</v>
+        <f>28.505675751544*1</f>
+        <v>28.505675751544</v>
       </c>
       <c r="AI29">
-        <f>4.4423209249399*1</f>
-        <v>4.4423209249399003</v>
+        <f>9.50189191723184*1</f>
+        <v>9.5018919172318395</v>
       </c>
       <c r="AJ29">
         <v>1</v>
@@ -7156,21 +7154,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>243</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>244</v>
       </c>
       <c r="C46" t="s">
-        <v>137</v>
+        <v>244</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -7179,10 +7177,10 @@
         <v>0</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -7197,7 +7195,7 @@
         <v>0</v>
       </c>
       <c r="N46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -7218,7 +7216,7 @@
         <v>0</v>
       </c>
       <c r="U46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V46">
         <v>0</v>
@@ -7245,30 +7243,30 @@
         <v>0</v>
       </c>
       <c r="AD46">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="AE46">
-        <v>182</v>
+        <v>455</v>
       </c>
       <c r="AF46">
-        <v>17.93452918934074</v>
+        <v>30.875608112397519</v>
       </c>
       <c r="AG46">
-        <v>15.65789473684211</v>
+        <v>17.625</v>
       </c>
       <c r="AH46">
-        <f>16.1998109067931*1</f>
-        <v>16.1998109067931</v>
+        <f>28.0265256860559*1</f>
+        <v>28.026525686055901</v>
       </c>
       <c r="AI46">
-        <f>3.23996241914661*1</f>
-        <v>3.2399624191466101</v>
+        <f>9.34217525621942*1</f>
+        <v>9.34217525621942</v>
       </c>
       <c r="AJ46">
         <v>1</v>
       </c>
       <c r="AK46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL46">
         <v>1</v>
@@ -8572,33 +8570,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>161</v>
+        <v>237</v>
       </c>
       <c r="B58" t="s">
-        <v>162</v>
+        <v>238</v>
       </c>
       <c r="C58" t="s">
-        <v>162</v>
+        <v>237</v>
       </c>
       <c r="D58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J58">
         <v>0</v>
@@ -8619,7 +8617,7 @@
         <v>0</v>
       </c>
       <c r="P58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q58">
         <v>0</v>
@@ -8631,7 +8629,7 @@
         <v>0</v>
       </c>
       <c r="T58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U58">
         <v>0</v>
@@ -8661,24 +8659,24 @@
         <v>0</v>
       </c>
       <c r="AD58">
-        <v>7</v>
+        <v>6.4</v>
       </c>
       <c r="AE58">
-        <v>273</v>
+        <v>425</v>
       </c>
       <c r="AF58">
-        <v>16.588861516277611</v>
+        <v>23.650306748466249</v>
       </c>
       <c r="AG58">
-        <v>22.737443581381559</v>
+        <v>20.974509829618551</v>
       </c>
       <c r="AH58">
-        <f>15.1435432849617*1</f>
-        <v>15.1435432849617</v>
+        <f>22.2945705438778*1</f>
+        <v>22.2945705438778</v>
       </c>
       <c r="AI58">
-        <f>3.78588582124042*1</f>
-        <v>3.7858858212404201</v>
+        <f>8.99500829962295*1</f>
+        <v>8.9950082996229508</v>
       </c>
       <c r="AJ58">
         <v>1</v>
@@ -8808,33 +8806,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>166</v>
+        <v>270</v>
       </c>
       <c r="B60" t="s">
-        <v>167</v>
+        <v>271</v>
       </c>
       <c r="C60" t="s">
-        <v>167</v>
+        <v>271</v>
       </c>
       <c r="D60" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60">
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J60">
         <v>0</v>
@@ -8855,7 +8853,7 @@
         <v>0</v>
       </c>
       <c r="P60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q60">
         <v>0</v>
@@ -8873,7 +8871,7 @@
         <v>0</v>
       </c>
       <c r="V60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W60">
         <v>0</v>
@@ -8897,30 +8895,30 @@
         <v>0</v>
       </c>
       <c r="AD60">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="AE60">
-        <v>276</v>
+        <v>510</v>
       </c>
       <c r="AF60">
-        <v>30.862335277903551</v>
+        <v>19.187854851488879</v>
       </c>
       <c r="AG60">
-        <v>10.89619823068201</v>
+        <v>21.17562146047139</v>
       </c>
       <c r="AH60">
-        <f>28.1734288816225*1</f>
-        <v>28.173428881622499</v>
+        <f>24.6632435473573*1</f>
+        <v>24.6632435473573</v>
       </c>
       <c r="AI60">
-        <f>7.04335722040564*1</f>
-        <v>7.0433572204056398</v>
+        <f>8.2692973018429*1</f>
+        <v>8.2692973018429008</v>
       </c>
       <c r="AJ60">
         <v>1</v>
       </c>
       <c r="AK60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL60">
         <v>1</v>
@@ -9870,33 +9868,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B69" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="C69" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="D69" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -9917,13 +9915,13 @@
         <v>0</v>
       </c>
       <c r="P69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q69">
         <v>0</v>
       </c>
       <c r="R69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S69">
         <v>0</v>
@@ -9959,24 +9957,24 @@
         <v>0</v>
       </c>
       <c r="AD69">
-        <v>4.5999999999999996</v>
+        <v>5.9</v>
       </c>
       <c r="AE69">
-        <v>344</v>
+        <v>276</v>
       </c>
       <c r="AF69">
-        <v>14.51006622148819</v>
+        <v>30.862335277903551</v>
       </c>
       <c r="AG69">
-        <v>13.64583333333333</v>
+        <v>10.89619823068201</v>
       </c>
       <c r="AH69">
-        <f>15.9421162383405*1</f>
-        <v>15.9421162383405</v>
+        <f>28.1734288816225*1</f>
+        <v>28.173428881622499</v>
       </c>
       <c r="AI69">
-        <f>3.18842296613119*1</f>
-        <v>3.1884229661311898</v>
+        <f>7.04335722040564*1</f>
+        <v>7.0433572204056398</v>
       </c>
       <c r="AJ69">
         <v>1</v>
@@ -12820,33 +12818,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>237</v>
+        <v>321</v>
       </c>
       <c r="B94" t="s">
-        <v>238</v>
+        <v>322</v>
       </c>
       <c r="C94" t="s">
-        <v>237</v>
+        <v>322</v>
       </c>
       <c r="D94" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E94">
         <v>0</v>
       </c>
       <c r="F94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94">
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J94">
         <v>0</v>
@@ -12879,7 +12877,7 @@
         <v>0</v>
       </c>
       <c r="T94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U94">
         <v>0</v>
@@ -12900,7 +12898,7 @@
         <v>0</v>
       </c>
       <c r="AA94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB94">
         <v>0</v>
@@ -12909,24 +12907,24 @@
         <v>0</v>
       </c>
       <c r="AD94">
-        <v>6.4</v>
+        <v>6.9</v>
       </c>
       <c r="AE94">
-        <v>425</v>
+        <v>709</v>
       </c>
       <c r="AF94">
-        <v>23.650306748466249</v>
+        <v>13.74648755351765</v>
       </c>
       <c r="AG94">
-        <v>20.974509829618551</v>
+        <v>16.09706473490759</v>
       </c>
       <c r="AH94">
-        <f>22.2945705438778*1</f>
-        <v>22.2945705438778</v>
+        <f>19.3019742833496*1</f>
+        <v>19.301974283349601</v>
       </c>
       <c r="AI94">
-        <f>8.99500829962295*1</f>
-        <v>8.9950082996229508</v>
+        <f>4.82549354378641*1</f>
+        <v>4.8254935437864104</v>
       </c>
       <c r="AJ94">
         <v>1</v>
@@ -13058,31 +13056,31 @@
     </row>
     <row r="96" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>241</v>
+        <v>337</v>
       </c>
       <c r="B96" t="s">
-        <v>242</v>
+        <v>338</v>
       </c>
       <c r="C96" t="s">
-        <v>242</v>
+        <v>338</v>
       </c>
       <c r="D96" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="F96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96">
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J96">
         <v>0</v>
@@ -13118,7 +13116,7 @@
         <v>0</v>
       </c>
       <c r="U96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V96">
         <v>0</v>
@@ -13139,36 +13137,36 @@
         <v>0</v>
       </c>
       <c r="AB96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC96">
         <v>0</v>
       </c>
       <c r="AD96">
-        <v>4.5999999999999996</v>
+        <v>7.8</v>
       </c>
       <c r="AE96">
-        <v>450</v>
+        <v>744</v>
       </c>
       <c r="AF96">
-        <v>12.56844477409547</v>
+        <v>22.256944444444429</v>
       </c>
       <c r="AG96">
-        <v>17.749994511662958</v>
+        <v>18.114035087719301</v>
       </c>
       <c r="AH96">
-        <f>28.2252863204879*1</f>
-        <v>28.2252863204879</v>
+        <f>22.3657224919037*1</f>
+        <v>22.3657224919037</v>
       </c>
       <c r="AI96">
-        <f>10.169834381442*1</f>
-        <v>10.169834381442</v>
+        <f>4.47314449838074*1</f>
+        <v>4.4731444983807398</v>
       </c>
       <c r="AJ96">
         <v>1</v>
       </c>
       <c r="AK96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL96">
         <v>1</v>
@@ -13176,13 +13174,13 @@
     </row>
     <row r="97" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>243</v>
+        <v>101</v>
       </c>
       <c r="B97" t="s">
-        <v>244</v>
+        <v>102</v>
       </c>
       <c r="C97" t="s">
-        <v>244</v>
+        <v>102</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
@@ -13200,7 +13198,7 @@
         <v>1</v>
       </c>
       <c r="I97" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J97">
         <v>0</v>
@@ -13209,7 +13207,7 @@
         <v>0</v>
       </c>
       <c r="L97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M97">
         <v>0</v>
@@ -13236,7 +13234,7 @@
         <v>0</v>
       </c>
       <c r="U97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V97">
         <v>0</v>
@@ -13263,30 +13261,30 @@
         <v>0</v>
       </c>
       <c r="AD97">
-        <v>5</v>
+        <v>6.9</v>
       </c>
       <c r="AE97">
-        <v>455</v>
+        <v>100</v>
       </c>
       <c r="AF97">
-        <v>30.875608112397519</v>
+        <v>30.73863803650563</v>
       </c>
       <c r="AG97">
-        <v>17.625</v>
+        <v>17.131578947368421</v>
       </c>
       <c r="AH97">
-        <f>28.0265256860559*1</f>
-        <v>28.026525686055901</v>
+        <f>25.5109831822738*1</f>
+        <v>25.510983182273801</v>
       </c>
       <c r="AI97">
-        <f>9.34217525621942*1</f>
-        <v>9.34217525621942</v>
+        <f>4.4423209249399*1</f>
+        <v>4.4423209249399003</v>
       </c>
       <c r="AJ97">
         <v>1</v>
       </c>
       <c r="AK97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL97">
         <v>1</v>
@@ -14354,137 +14352,137 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>264</v>
+        <v>92</v>
       </c>
       <c r="B107" t="s">
-        <v>265</v>
+        <v>93</v>
       </c>
       <c r="C107" t="s">
-        <v>265</v>
+        <v>94</v>
       </c>
       <c r="D107" t="s">
+        <v>3</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107" t="s">
+        <v>13</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>1</v>
+      </c>
+      <c r="M107">
+        <v>0</v>
+      </c>
+      <c r="N107">
+        <v>0</v>
+      </c>
+      <c r="O107">
+        <v>0</v>
+      </c>
+      <c r="P107">
+        <v>0</v>
+      </c>
+      <c r="Q107">
+        <v>0</v>
+      </c>
+      <c r="R107">
+        <v>0</v>
+      </c>
+      <c r="S107">
+        <v>0</v>
+      </c>
+      <c r="T107">
+        <v>0</v>
+      </c>
+      <c r="U107">
+        <v>0</v>
+      </c>
+      <c r="V107">
+        <v>0</v>
+      </c>
+      <c r="W107">
+        <v>0</v>
+      </c>
+      <c r="X107">
+        <v>0</v>
+      </c>
+      <c r="Y107">
+        <v>0</v>
+      </c>
+      <c r="Z107">
+        <v>0</v>
+      </c>
+      <c r="AA107">
+        <v>0</v>
+      </c>
+      <c r="AB107">
+        <v>0</v>
+      </c>
+      <c r="AC107">
+        <v>0</v>
+      </c>
+      <c r="AD107">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AE107">
+        <v>92</v>
+      </c>
+      <c r="AF107">
+        <v>21.700584998227729</v>
+      </c>
+      <c r="AG107">
+        <v>19.416666666666671</v>
+      </c>
+      <c r="AH107">
+        <f>24.8022480203325*1</f>
+        <v>24.802248020332499</v>
+      </c>
+      <c r="AI107">
+        <f>4.09094795889088*1</f>
+        <v>4.0909479588908804</v>
+      </c>
+      <c r="AJ107">
+        <v>1</v>
+      </c>
+      <c r="AK107">
+        <v>1</v>
+      </c>
+      <c r="AL107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>161</v>
+      </c>
+      <c r="B108" t="s">
+        <v>162</v>
+      </c>
+      <c r="C108" t="s">
+        <v>162</v>
+      </c>
+      <c r="D108" t="s">
         <v>5</v>
       </c>
-      <c r="E107">
-        <v>0</v>
-      </c>
-      <c r="F107">
-        <v>0</v>
-      </c>
-      <c r="G107">
-        <v>1</v>
-      </c>
-      <c r="H107">
-        <v>0</v>
-      </c>
-      <c r="I107" t="s">
-        <v>23</v>
-      </c>
-      <c r="J107">
-        <v>0</v>
-      </c>
-      <c r="K107">
-        <v>0</v>
-      </c>
-      <c r="L107">
-        <v>0</v>
-      </c>
-      <c r="M107">
-        <v>0</v>
-      </c>
-      <c r="N107">
-        <v>0</v>
-      </c>
-      <c r="O107">
-        <v>0</v>
-      </c>
-      <c r="P107">
-        <v>0</v>
-      </c>
-      <c r="Q107">
-        <v>0</v>
-      </c>
-      <c r="R107">
-        <v>0</v>
-      </c>
-      <c r="S107">
-        <v>0</v>
-      </c>
-      <c r="T107">
-        <v>0</v>
-      </c>
-      <c r="U107">
-        <v>0</v>
-      </c>
-      <c r="V107">
-        <v>1</v>
-      </c>
-      <c r="W107">
-        <v>0</v>
-      </c>
-      <c r="X107">
-        <v>0</v>
-      </c>
-      <c r="Y107">
-        <v>0</v>
-      </c>
-      <c r="Z107">
-        <v>0</v>
-      </c>
-      <c r="AA107">
-        <v>0</v>
-      </c>
-      <c r="AB107">
-        <v>0</v>
-      </c>
-      <c r="AC107">
-        <v>0</v>
-      </c>
-      <c r="AD107">
-        <v>8</v>
-      </c>
-      <c r="AE107">
-        <v>497</v>
-      </c>
-      <c r="AF107">
-        <v>34.804013156453273</v>
-      </c>
-      <c r="AG107">
-        <v>24.474696445768739</v>
-      </c>
-      <c r="AH107">
-        <f>28.505675751544*1</f>
-        <v>28.505675751544</v>
-      </c>
-      <c r="AI107">
-        <f>9.50189191723184*1</f>
-        <v>9.5018919172318395</v>
-      </c>
-      <c r="AJ107">
-        <v>1</v>
-      </c>
-      <c r="AK107">
-        <v>1</v>
-      </c>
-      <c r="AL107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>266</v>
-      </c>
-      <c r="B108" t="s">
-        <v>267</v>
-      </c>
-      <c r="C108" t="s">
-        <v>267</v>
-      </c>
-      <c r="D108" t="s">
-        <v>6</v>
-      </c>
       <c r="E108">
         <v>0</v>
       </c>
@@ -14492,13 +14490,13 @@
         <v>0</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J108">
         <v>0</v>
@@ -14519,7 +14517,7 @@
         <v>0</v>
       </c>
       <c r="P108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q108">
         <v>0</v>
@@ -14537,7 +14535,7 @@
         <v>0</v>
       </c>
       <c r="V108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W108">
         <v>0</v>
@@ -14561,24 +14559,24 @@
         <v>0</v>
       </c>
       <c r="AD108">
-        <v>14.4</v>
+        <v>7</v>
       </c>
       <c r="AE108">
-        <v>499</v>
+        <v>273</v>
       </c>
       <c r="AF108">
-        <v>47.510204081632637</v>
+        <v>16.588861516277611</v>
       </c>
       <c r="AG108">
-        <v>47.672769754447117</v>
+        <v>22.737443581381559</v>
       </c>
       <c r="AH108">
-        <f>55.5244687021735*1</f>
-        <v>55.5244687021735</v>
+        <f>15.1435432849617*1</f>
+        <v>15.1435432849617</v>
       </c>
       <c r="AI108">
-        <f>18.5367479360317*1</f>
-        <v>18.536747936031698</v>
+        <f>3.78588582124042*1</f>
+        <v>3.7858858212404201</v>
       </c>
       <c r="AJ108">
         <v>1</v>
@@ -14710,13 +14708,13 @@
     </row>
     <row r="110" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>270</v>
+        <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>271</v>
+        <v>57</v>
       </c>
       <c r="C110" t="s">
-        <v>271</v>
+        <v>57</v>
       </c>
       <c r="D110" t="s">
         <v>4</v>
@@ -14734,10 +14732,10 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K110">
         <v>0</v>
@@ -14773,7 +14771,7 @@
         <v>0</v>
       </c>
       <c r="V110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W110">
         <v>0</v>
@@ -14797,30 +14795,30 @@
         <v>0</v>
       </c>
       <c r="AD110">
-        <v>5.5</v>
+        <v>5.6</v>
       </c>
       <c r="AE110">
-        <v>510</v>
+        <v>18</v>
       </c>
       <c r="AF110">
-        <v>19.187854851488879</v>
+        <v>18.217404566884401</v>
       </c>
       <c r="AG110">
-        <v>21.17562146047139</v>
+        <v>19.065496153059801</v>
       </c>
       <c r="AH110">
-        <f>24.6632435473573*1</f>
-        <v>24.6632435473573</v>
+        <f>20.4859392927446*1</f>
+        <v>20.4859392927446</v>
       </c>
       <c r="AI110">
-        <f>8.2692973018429*1</f>
-        <v>8.2692973018429008</v>
+        <f>3.61005959840199*1</f>
+        <v>3.6100595984019899</v>
       </c>
       <c r="AJ110">
         <v>1</v>
       </c>
       <c r="AK110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL110">
         <v>1</v>
@@ -17658,33 +17656,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>321</v>
+        <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>322</v>
+        <v>137</v>
       </c>
       <c r="C135" t="s">
-        <v>322</v>
+        <v>137</v>
       </c>
       <c r="D135" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F135">
         <v>0</v>
       </c>
       <c r="G135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H135">
         <v>0</v>
       </c>
       <c r="I135" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="J135">
         <v>0</v>
@@ -17699,7 +17697,7 @@
         <v>0</v>
       </c>
       <c r="N135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O135">
         <v>0</v>
@@ -17738,7 +17736,7 @@
         <v>0</v>
       </c>
       <c r="AA135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB135">
         <v>0</v>
@@ -17747,24 +17745,24 @@
         <v>0</v>
       </c>
       <c r="AD135">
-        <v>6.9</v>
+        <v>4.2</v>
       </c>
       <c r="AE135">
-        <v>709</v>
+        <v>182</v>
       </c>
       <c r="AF135">
-        <v>13.74648755351765</v>
+        <v>17.93452918934074</v>
       </c>
       <c r="AG135">
-        <v>16.09706473490759</v>
+        <v>15.65789473684211</v>
       </c>
       <c r="AH135">
-        <f>19.3019742833496*1</f>
-        <v>19.301974283349601</v>
+        <f>16.1998109067931*1</f>
+        <v>16.1998109067931</v>
       </c>
       <c r="AI135">
-        <f>4.82549354378641*1</f>
-        <v>4.8254935437864104</v>
+        <f>3.23996241914661*1</f>
+        <v>3.2399624191466101</v>
       </c>
       <c r="AJ135">
         <v>1</v>
@@ -18602,33 +18600,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>337</v>
+        <v>185</v>
       </c>
       <c r="B143" t="s">
-        <v>338</v>
+        <v>186</v>
       </c>
       <c r="C143" t="s">
-        <v>338</v>
+        <v>186</v>
       </c>
       <c r="D143" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E143">
         <v>0</v>
       </c>
       <c r="F143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G143">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H143">
         <v>0</v>
       </c>
       <c r="I143" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="J143">
         <v>0</v>
@@ -18655,7 +18653,7 @@
         <v>0</v>
       </c>
       <c r="R143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S143">
         <v>0</v>
@@ -18685,30 +18683,30 @@
         <v>0</v>
       </c>
       <c r="AB143">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC143">
         <v>0</v>
       </c>
       <c r="AD143">
-        <v>7.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AE143">
-        <v>744</v>
+        <v>344</v>
       </c>
       <c r="AF143">
-        <v>22.256944444444429</v>
+        <v>14.51006622148819</v>
       </c>
       <c r="AG143">
-        <v>18.114035087719301</v>
+        <v>13.64583333333333</v>
       </c>
       <c r="AH143">
-        <f>22.3657224919037*1</f>
-        <v>22.3657224919037</v>
+        <f>15.9421162383405*1</f>
+        <v>15.9421162383405</v>
       </c>
       <c r="AI143">
-        <f>4.47314449838074*1</f>
-        <v>4.4731444983807398</v>
+        <f>3.18842296613119*1</f>
+        <v>3.1884229661311898</v>
       </c>
       <c r="AJ143">
         <v>1</v>

</xml_diff>